<commit_message>
Ultimos cambios de página
</commit_message>
<xml_diff>
--- a/public/files/Archivo_definitivo.xlsx
+++ b/public/files/Archivo_definitivo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zurie\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BEEBD38-5BBA-46BC-89DB-124ED82F05A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0791DDF3-1193-4B48-B1CB-D3DC2E0E9685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A3A7B47-804D-4526-9844-BE36CD6CBBAB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Funciones</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Edecán</t>
+  </si>
+  <si>
+    <t>Limpieza</t>
+  </si>
+  <si>
+    <t>Otros</t>
   </si>
 </sst>
 </file>
@@ -448,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96148FC8-C129-454B-A7F6-732528E7B734}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A1299" workbookViewId="0">
+      <selection activeCell="H1307" sqref="H1307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,14 +488,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC7D1301-1496-4ECC-ADE4-99557D1D1633}">
           <x14:formula1>
-            <xm:f>Hoja2!$A$2:$A$3</xm:f>
+            <xm:f>Hoja2!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D2</xm:sqref>
+          <xm:sqref>D2:D1300</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -496,10 +506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D9C0B4-8F6E-4A35-8522-E4AE0C925AF1}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,6 +529,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ultimos cambios de archivo xlxs
</commit_message>
<xml_diff>
--- a/public/files/Archivo_definitivo.xlsx
+++ b/public/files/Archivo_definitivo.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zurie\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00EC3CE-DE43-42AD-B73F-EEF1A00B9ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF86ED8-BC04-4782-84AC-F4C95BA29EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A3A7B47-804D-4526-9844-BE36CD6CBBAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,16 +95,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -112,14 +150,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -455,36 +531,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96148FC8-C129-454B-A7F6-732528E7B734}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1307" sqref="H1307"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="27" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" style="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F2" s="1"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
arreglo de archivo patrocinadores
</commit_message>
<xml_diff>
--- a/public/files/Archivo_definitivo.xlsx
+++ b/public/files/Archivo_definitivo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zurie\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF86ED8-BC04-4782-84AC-F4C95BA29EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DCE1EF-A64D-4C71-9A61-A5386D1A8397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A3A7B47-804D-4526-9844-BE36CD6CBBAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Funciones</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Otros</t>
+  </si>
+  <si>
+    <t>Patrocinadores</t>
   </si>
 </sst>
 </file>
@@ -533,7 +536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96148FC8-C129-454B-A7F6-732528E7B734}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -582,7 +587,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC7D1301-1496-4ECC-ADE4-99557D1D1633}">
           <x14:formula1>
-            <xm:f>Hoja2!$A$2:$A$6</xm:f>
+            <xm:f>Hoja2!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1300</xm:sqref>
         </x14:dataValidation>
@@ -594,13 +599,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D9C0B4-8F6E-4A35-8522-E4AE0C925AF1}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -629,6 +637,11 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>